<commit_message>
maj qualité images & producs/supplements
</commit_message>
<xml_diff>
--- a/quizz-complements-json.xlsx
+++ b/quizz-complements-json.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7be2adeba9231ed7/Documents/_work/AltCare/_projets/mental-booster/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\server\AltCare\mental-booster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{8DFEB29C-4E02-48C2-A77F-59C6D60F7D94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{37BD3659-3BF4-4798-95B9-B61C5C9B9AE3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482DA35B-813B-4737-8817-2E1237F2C2A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{94638537-CEAC-4A25-B219-AE2EAB8581B2}"/>
   </bookViews>
@@ -46,9 +46,6 @@
 Le 5-HTP est extrait des graines de Griffonia simplicifolia, une plante africaine. Il est converti en neurotransmetteur, la sérotonine (5-hydroxytryptamine, 5-HT), laquelle permet la transmission de l’influx nerveux dans le cerveau et la régulation de l’humeur, de l’anxiété, de l’appétit et du sommeil. Le 5-HTP est considéré comme antidépresseur au même titre que les antidépresseurs classiques.</t>
   </si>
   <si>
-    <t>5-HTP.png</t>
-  </si>
-  <si>
     <t>Acétylcholine</t>
   </si>
   <si>
@@ -76,17 +73,11 @@
 Par ailleurs, certaines données suggèrent que les bacosides A et B du bacopa peuvent faciliter la capacité d'apprentissage, la mémoire et les performances cognitives. Les mécanismes possibles d'amélioration cognitive comprennent la modulation de la libération d'acétylcholine, l'activité de la choline acétylase et la liaison aux récepteurs cholinergiques.</t>
   </si>
   <si>
-    <t>bacopa.jpeg</t>
-  </si>
-  <si>
     <t>Choline</t>
   </si>
   <si>
     <t>La choline est un nutriment essentiel apparenté aux vitamines hydrosolubles du groupe B (folate, pyridoxine et vitamine B12), et à la méthionine, un acide aminé essentiel. La choline est un composant des membranes cellulaires et est nécessaire à la synthèse des phospholipides. C'est aussi le précurseur de l'acétylcholine et participe au développement du cerveau, à la neurotransmission et à la signalisation. La choline est synthétisée dans l'organisme et consommée dans l'alimentation. La plus grande source alimentaire de choline est le jaune d'œuf. D'autres aliments qui fournissent de grandes quantités de choline sont le foie, les viandes musculaires, le poisson, les noix, les haricots, les pois, les germes de blé, les épinards et autres. Un régime alimentaire typique fournit 200-600 mg de choline par jour. _x000D_
 La choline est principalement utilisée pour ses propriétés de stimulation cognitive (transformation en acétylcholine, le neurotransmetteur d'apprentissage), ou comme agent de santé du foie, capable de réduire l'accumulation de graisse dans le foie.</t>
-  </si>
-  <si>
-    <t>Choline.jpg</t>
   </si>
   <si>
     <t>DHA (Docosahexaenoic acid)</t>
@@ -95,9 +86,6 @@
     <t xml:space="preserve">Le DHA (acide docosahexaénoïque) est un acide gras polyinsaturé oméga-3 à longue chaîne, de 22 carbones. On le trouve dans certains types de microalgues marines, ainsi que dans les tissus de mammifères marins et de poissons gras (thon, saumon). Le DHA est également présent dans les huiles de foie de poisson et dans les produits à base d'huile de poisson. Le DHA ne peut pas être synthétisé de novo (sans précurseur) par les mammifères. Une partie du DHA nécessaire à l'être humain est synthétisé à partir d'acide alpha-linolénique (ALA). Le DHA peut être converti en EPA (acide eicosapentaénoïque) chez l'homme. _x000D_
 Le DHA contribue au développement normal du fœtus, des nourrissons et des enfants, notamment lorsque la mère est atopique. Il contribue également au maintien des fonctions normales du cerveau, d’une vision normale, d'une pression sanguine normale ainsi que des taux de triglycérides normaux chez les adultes._x000D_
 Le DHA est considéré comme important pour le fonctionnement normal des neurones et pourrait jouer un rôle clé dans le développement structurel des membranes neuronales et synaptiques.  Le DHA s'accumule rapidement dans le cerveau humain au cours du troisième trimestre de la grossesse et au début de la période postnatale. L'accumulation de DHA et d'autres acides gras à cette période entraîne un développement et une croissance rapides des tissus cérébraux. </t>
-  </si>
-  <si>
-    <t>Docosahexaenoic_acid.png</t>
   </si>
   <si>
     <t>GABA</t>
@@ -147,9 +135,6 @@
 Une alimentation pauvre en acides gras oméga-3 peut affecter la composition en acides gras des cellules du système nerveux central et altérer la fonction neurale, y compris le développement intellectuel ou cognitif. Des niveaux réduits d’acides gras oméga-3 ont été rapportés chez les personnes atteintes de schizophrénie, et il est suggéré que le trouble est en rapport avec un dysfonctionnement du métabolisme des acides gras. En effet, les acides gras oméga-3 peuvent altérer la fluidité de la membrane et la réponse des récepteurs lorsqu'ils sont incorporés dans les membranes cellulaires et peuvent interagir avec les systèmes dopaminergiques et sérotonergiques.</t>
   </si>
   <si>
-    <t>Huile de poisson.jpg</t>
-  </si>
-  <si>
     <t>L-glutamine</t>
   </si>
   <si>
@@ -172,9 +157,6 @@
 Les sources alimentaires de magnésium comprennent les légumineuses, les grains entiers, les légumes (en particulier le brocoli, la courge et les légumes à feuilles vertes), les graines et les noix (en particulier les amandes). Les autres sources comprennent les produits laitiers, les viandes, le chocolat et le café._x000D_
 Une relation entre le magnésium et les états dépressifs a été établie. Le magnésium joue un rôle clé dans l'activité des systèmes psychoneuroendocriniens impliqués dans la physiopathologie de la dépression. Par exemple, tous les éléments de l'axe hypothalamo-hypophyso-surrénalien sont sensibles à l'action du Mg (l'axe hypothalamo-hypophyso-surrénalien est constitué des interactions entre l'hypothalamus, l'hypophyse et les glandes surrénales, il contrôle les réponses au stress). Il a également été démontré que le magnésium atténue la libération de l'hormone adrénocorticotrophe (hormone secrétée par l'hypophyse et stimule la glande corticosurrénale) et peut influencer le passage des corticostéroïdes au cerveau à travers la barrière hémato-encéphalique._x000D_
 Les carences en magnésium sont courantes dans les pays développés.</t>
-  </si>
-  <si>
-    <t>Magnesium.png</t>
   </si>
   <si>
     <t>Mélatonine</t>
@@ -194,9 +176,6 @@
 Il a été proposé que la mélatonine puisse réduire les dommages neurologiques secondaires à un accident vasculaire cérébral, en raison de ses propriétés antioxydantes._x000D_
 D'autre part, la mélatonine semble efficace dans la maladie d'Alzheimer. Des études en laboratoire montrent qu'elle atténuait la phosphorylation de la protéine tau (un peptide dont l'agrégation est un signe de la maladie d'Alzheimer), prévenait  la neuroinflammation, et atténuait le dysfonctionnement mitochondrial médié par la bêta-amyloïde (protéine présente dans les neurones et dont l'agrégation est un signe de la maladie d'Alzheimer) . De plus, des preuves in vitro suggèrent que la mélatonine pourrait inhiber les processus biochimiques impliqués dans le développement des plaques myéloïdes trouvées dans le cerveau des patients atteints de la maladie d'Alzheimer ; cependant, la signification clinique n'est pas claire._x000D_
 La mélatonine semble également efficace pour diminuer les céphalées. Selon une étude, plusieurs mécanismes sont possibles dont l'élimination des radicaux libres toxiques, la réduction des cytokines pro-inflammatoires, l'activité de l'oxyde nitrique synthase et l'inhibition de la libération de dopamine, la stabilisation de la membrane, la potentialisation du GABA et de l'analgésie opioïde et la protection de la neurotoxicité du glutamate.</t>
-  </si>
-  <si>
-    <t>Mélatonine.png</t>
   </si>
   <si>
     <t>Millepertuis</t>
@@ -245,9 +224,6 @@
 La Tyrosine est efficace pour stimuler les fonctions cognitives. Elle est particulièrement utile pour maintenir les performances cognitives et la mémoire dans des conditions de stress.</t>
   </si>
   <si>
-    <t>Tyrosine.jpg</t>
-  </si>
-  <si>
     <t>Valériane</t>
   </si>
   <si>
@@ -273,9 +249,6 @@
 La thiamine est essentielle au métabolisme énergétique normal, au fonctionnement normal du cœur, au fonctionnement du système nerveux et semble indispensable à la mémorisation ainsi qu’aux facultés intellectuelles.  La TPP intervient également dans la décarboxylation oxydative du pyruvate qui est  une étape nécessaire à la formation d'acétylcholine (un neurotransmetteur). </t>
   </si>
   <si>
-    <t>B1.png</t>
-  </si>
-  <si>
     <t>Vitamine B3</t>
   </si>
   <si>
@@ -286,9 +259,6 @@
 Les grands déficits en vitamine B3 sont la cause du syndrome pellagreux. La pellagre est une affection essentiellement cutanée avec un érythème douloureux étendu aux parties exposées à la lumière, parfois accompagné d’une stomatite et d’une glossite, et souvent d’une asthénie physique et psychique intense avec mélancolie délirante à tendance dépressive, enfin d’atteintes digestives avec diarrhées et plus tardivement de troubles neurologiques sensitifs et douloureux.</t>
   </si>
   <si>
-    <t>B3.png</t>
-  </si>
-  <si>
     <t>Vitamine B5</t>
   </si>
   <si>
@@ -297,9 +267,6 @@
 La  vitamine B5 contribue au métabolisme énergétique normal, aux capacités intellectuelles normales, à la synthèse des hormones stéroïdiennes (hormones du stress et hormones sexuelles), de la vitamine D et de certains messagers chimiques du cerveau (neurotransmetteurs) et elle contribue à la réduction de la fatigue. </t>
   </si>
   <si>
-    <t>B5.png</t>
-  </si>
-  <si>
     <t>Vitamine B6</t>
   </si>
   <si>
@@ -314,18 +281,12 @@
 La vitamine B6 contribue au au métabolisme énergétique normal, au fonctionnement normal du système nerveux, à la synthèse normale de la cystéine et au métabolisme normal de l’homocystéine, à la réduction de la fatigue, au métabolisme normal du glycogène et des protéines, aux fonctions mentales normales, à la formation des globules rouges, au fonctionnement normal du système immunitaire et à la régulation de l’activité hormonale. </t>
   </si>
   <si>
-    <t>B6.png</t>
-  </si>
-  <si>
     <t>Vitamine B12</t>
   </si>
   <si>
     <t>La vitamine B12 ou cobalamine est une vitamine essentielle hydrosoluble. Elle est exclusivement synthétisée par des bactéries et elle est présente dans les aliments d’origine animale (tels que le poisson, les crustacés, la viande, les œufs et les produits laitiers), liée à des protéines. Les sources végétales alimentaires sont naturellement dépourvues de vitamine B12 biodisponible. Certains produits végétaux ayant subi une fermentation bactérienne, tels que la bière, peuvent contenir de la cobalamine, mais en quantité très faible. _x000D_
 La méthylcobalamine, une forme de vitaline B12, semble améliorer la vigilance et réduire le temps de sommeil chez les sujets ayant un sommeil normal, peut-être en agissant sur la mélatonine. D'autre part, certaines recherches montrent que des taux élevés d'homocystéine sérique et des taux faibles de folate et de vitamine B12 peuvent être associés à un déclin cognitif et à une démence._x000D_
 La supplémentation en vitamine B12 peut améliorer les symptômes du syndrome de fatigue chronique en corrigeant les anomalies des globules rouges et en améliorant l'apport d'oxygène aux tissus.</t>
-  </si>
-  <si>
-    <t>B12.png</t>
   </si>
   <si>
     <t>dMin</t>
@@ -368,9 +329,6 @@
 Par voie orale, le Mucuna pruriens est utilisé pour la maladie de Parkinson, l'anxiété, en cas de douleur, de fièvre, et pour améliorer la libido.</t>
   </si>
   <si>
-    <t>Mucuna pruriens.jpg</t>
-  </si>
-  <si>
     <t>Vitamine B2</t>
   </si>
   <si>
@@ -389,9 +347,6 @@
 La riboflavine est nécessaire au métabolisme des acides gras essentiels. De plus, la riboflavine est impliquée dans la formation de myéline à la fois dans le système nerveux central et le système nerveux périphérique. Chez les patients déficients en riboflavine, les composants des nerfs, y compris les lipides, sont réduits, ce qui peut affecter le développement du cerveau. </t>
   </si>
   <si>
-    <t>B2.png</t>
-  </si>
-  <si>
     <t>Vitamine B8</t>
   </si>
   <si>
@@ -405,9 +360,6 @@
 enzyme de leur biosynthèse._x000D_
 Il existe deux isomères, l'alpha biotine, se trouvant préférentiellement dans le jaune d’œuf, et la bêta biotine, se trouvant dans le foie et les rognons, un peu moins dans les légumes secs, les champignons, le chocolat et les levures. Notre flore intestinale en fabrique un peu. _x000D_
 La vitamine B8 contribue au métabolisme énergétique normal, au fonctionnement normal du système nerveux, au maintien de cheveux, d’une peau et de muqueuses normales, au métabolisme normal des aliments et aux fonctions mentales normales.</t>
-  </si>
-  <si>
-    <t>B8.png</t>
   </si>
   <si>
     <t>Vitamine B9</t>
@@ -430,9 +382,6 @@
 Dans la population générale, les personnes ayant un faible niveau d'acide folique ou un apport alimentaire faible en folates ont un risque plus élevé de développer une dépression. De plus, de faibles niveaux de folate ont été liés à une mauvaise réponse au traitement antidépresseur. Le rôle exact de l'acide folique dans la dépression n'est pas encore connu. Mais il est nécessaire pour la reméthylation de l'homocystéine en méthionine et pour la conversion de la s-adénosylméthionine (SAMe). Il intervient également dans la méthylation de la tétrahydrobioptérine, un cofacteur essentiel des enzymes hydroxylases impliquées dans la production de neurotransmetteurs tels que la sérotonine.</t>
   </si>
   <si>
-    <t>B9.png</t>
-  </si>
-  <si>
     <t>1 mg</t>
   </si>
   <si>
@@ -452,9 +401,6 @@
 De plus, la déplétion alimentaire en L-tryptophane a été associée à une rechute de la boulimie et à une détérioration des symptômes de la schizophrénie.</t>
   </si>
   <si>
-    <t>L-Tryptophane.png</t>
-  </si>
-  <si>
     <t>Zinc</t>
   </si>
   <si>
@@ -474,9 +420,6 @@
 Dans la maladie d'Alzheimer, Le zinc semble jouer un rôle protecteur grâce à ses propriétés antioxydantes, mais d'autre part, il semble contribuer à l'agrégation du bêta-amyloïde (petite protéine dont l'agrégat est un des signes caractéristiques de l’Alzheimer).</t>
   </si>
   <si>
-    <t>Zinc.png</t>
-  </si>
-  <si>
     <t>title</t>
   </si>
   <si>
@@ -487,6 +430,63 @@
   </si>
   <si>
     <t>neuro</t>
+  </si>
+  <si>
+    <t>choline.jpg</t>
+  </si>
+  <si>
+    <t>docosahexaenoic_acid.png</t>
+  </si>
+  <si>
+    <t>b1.png</t>
+  </si>
+  <si>
+    <t>b12.png</t>
+  </si>
+  <si>
+    <t>b5.png</t>
+  </si>
+  <si>
+    <t>tyrosine.jpg</t>
+  </si>
+  <si>
+    <t>mucuna-pruriens.jpg</t>
+  </si>
+  <si>
+    <t>b2.png</t>
+  </si>
+  <si>
+    <t>b3.png</t>
+  </si>
+  <si>
+    <t>b6.png</t>
+  </si>
+  <si>
+    <t>bacopa.jpg</t>
+  </si>
+  <si>
+    <t>b8.png</t>
+  </si>
+  <si>
+    <t>b9.png</t>
+  </si>
+  <si>
+    <t>melatonine.png</t>
+  </si>
+  <si>
+    <t>huile-poisson.jpg</t>
+  </si>
+  <si>
+    <t>magnesium.png</t>
+  </si>
+  <si>
+    <t>5-htp.png</t>
+  </si>
+  <si>
+    <t>l-tryptophane.png</t>
+  </si>
+  <si>
+    <t>zinc.png</t>
   </si>
 </sst>
 </file>
@@ -574,16 +574,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E2920D29-068E-4443-AD3F-5B7278DCD815}" name="Tableau2" displayName="Tableau2" ref="A1:G39" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E2920D29-068E-4443-AD3F-5B7278DCD815}" name="Tableau2" displayName="Tableau2" ref="A1:G39" totalsRowShown="0" headerRowDxfId="8" dataDxfId="0">
   <autoFilter ref="A1:G39" xr:uid="{9B6BC5F5-B9AA-4642-AE00-C60A9B12B6CB}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{BCE2BCBC-B9E5-47FC-8546-26A7543594A3}" name="neuro" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{F5959514-144E-4EFC-8AD4-5E9033096356}" name="title" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{DCCB1E6E-A91D-4B74-85DF-A2AE6E8E2E98}" name="dMin" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{0A9F51FF-51B8-4C32-B8BF-4F35591BAFCC}" name="dMoy" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{57DE3885-09E2-44D4-BECA-718E881AFF1B}" name="dMax" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{F4E92262-E3A7-4998-9228-C099404B936C}" name="desc" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{B564A475-A0B7-4A02-A8DA-EE6F45B025BB}" name="file" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{BCE2BCBC-B9E5-47FC-8546-26A7543594A3}" name="neuro" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{F5959514-144E-4EFC-8AD4-5E9033096356}" name="title" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{DCCB1E6E-A91D-4B74-85DF-A2AE6E8E2E98}" name="dMin" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{0A9F51FF-51B8-4C32-B8BF-4F35591BAFCC}" name="dMoy" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{57DE3885-09E2-44D4-BECA-718E881AFF1B}" name="dMax" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{F4E92262-E3A7-4998-9228-C099404B936C}" name="desc" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{B564A475-A0B7-4A02-A8DA-EE6F45B025BB}" name="file" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -906,33 +906,33 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>2</v>
@@ -944,44 +944,44 @@
         <v>4</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>18</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>15</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>2</v>
@@ -990,18 +990,18 @@
         <v>3</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>3</v>
@@ -1010,67 +1010,67 @@
         <v>4</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>67</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>2</v>
@@ -1082,90 +1082,90 @@
         <v>4</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>81</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>73</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>60</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>2</v>
@@ -1174,21 +1174,21 @@
         <v>3</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>2</v>
@@ -1197,41 +1197,41 @@
         <v>3</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>2</v>
@@ -1243,67 +1243,67 @@
         <v>4</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>67</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>2</v>
@@ -1312,205 +1312,205 @@
         <v>4</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>70</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>73</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>78</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>81</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>67</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>48</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>2</v>
@@ -1519,41 +1519,41 @@
         <v>4</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>70</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>78</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>3</v>
@@ -1562,21 +1562,21 @@
         <v>4</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>2</v>
@@ -1588,10 +1588,10 @@
         <v>4</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1599,22 +1599,22 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>35</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1622,22 +1622,22 @@
         <v>0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>42</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1645,22 +1645,22 @@
         <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>78</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1668,7 +1668,7 @@
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>3</v>
@@ -1677,13 +1677,13 @@
         <v>4</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1691,22 +1691,22 @@
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1714,22 +1714,22 @@
         <v>0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>48</v>
+        <v>121</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1752,7 +1752,7 @@
         <v>5</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>6</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1760,22 +1760,22 @@
         <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1783,22 +1783,22 @@
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
maj products pour filtrage
</commit_message>
<xml_diff>
--- a/quizz-complements-json.xlsx
+++ b/quizz-complements-json.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\server\AltCare\mental-booster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482DA35B-813B-4737-8817-2E1237F2C2A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9213F31-4BD7-4D5F-87C9-13754714D127}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{94638537-CEAC-4A25-B219-AE2EAB8581B2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="128">
   <si>
     <t>Sérotonine</t>
   </si>
@@ -487,6 +487,9 @@
   </si>
   <si>
     <t>zinc.png</t>
+  </si>
+  <si>
+    <t>supplementId</t>
   </si>
 </sst>
 </file>
@@ -525,18 +528,20 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -574,16 +579,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E2920D29-068E-4443-AD3F-5B7278DCD815}" name="Tableau2" displayName="Tableau2" ref="A1:G39" totalsRowShown="0" headerRowDxfId="8" dataDxfId="0">
-  <autoFilter ref="A1:G39" xr:uid="{9B6BC5F5-B9AA-4642-AE00-C60A9B12B6CB}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{BCE2BCBC-B9E5-47FC-8546-26A7543594A3}" name="neuro" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{F5959514-144E-4EFC-8AD4-5E9033096356}" name="title" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{DCCB1E6E-A91D-4B74-85DF-A2AE6E8E2E98}" name="dMin" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{0A9F51FF-51B8-4C32-B8BF-4F35591BAFCC}" name="dMoy" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{57DE3885-09E2-44D4-BECA-718E881AFF1B}" name="dMax" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{F4E92262-E3A7-4998-9228-C099404B936C}" name="desc" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{B564A475-A0B7-4A02-A8DA-EE6F45B025BB}" name="file" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E2920D29-068E-4443-AD3F-5B7278DCD815}" name="Tableau2" displayName="Tableau2" ref="A1:H39" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="A1:H39" xr:uid="{9B6BC5F5-B9AA-4642-AE00-C60A9B12B6CB}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{BCE2BCBC-B9E5-47FC-8546-26A7543594A3}" name="neuro" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{F5959514-144E-4EFC-8AD4-5E9033096356}" name="title" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{DCCB1E6E-A91D-4B74-85DF-A2AE6E8E2E98}" name="dMin" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{0A9F51FF-51B8-4C32-B8BF-4F35591BAFCC}" name="dMoy" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{57DE3885-09E2-44D4-BECA-718E881AFF1B}" name="dMax" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{F4E92262-E3A7-4998-9228-C099404B936C}" name="desc" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{B564A475-A0B7-4A02-A8DA-EE6F45B025BB}" name="file" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{2C46B663-473A-4306-BA4B-ACD35C446C06}" name="supplementId" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -886,25 +892,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17CE438A-0712-489D-A5ED-038772CD7804}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G39"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="34" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="80.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="1"/>
+    <col min="6" max="6" width="36.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="25" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.7109375" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>107</v>
       </c>
@@ -926,13 +934,16 @@
       <c r="G1" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>2</v>
@@ -943,14 +954,17 @@
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>15</v>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -966,37 +980,43 @@
       <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H4" s="2">
         <v>3</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1012,16 +1032,19 @@
       <c r="E5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>20</v>
@@ -1035,37 +1058,43 @@
       <c r="E6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>58</v>
+      <c r="F7" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="H7" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1081,566 +1110,641 @@
       <c r="E8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="1" t="s">
         <v>26</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>75</v>
+        <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>76</v>
+        <v>8</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>68</v>
+        <v>29</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="H9" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>57</v>
+        <v>2</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>62</v>
+        <v>4</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+      <c r="H10" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>52</v>
+      <c r="F11" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="H11" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H12" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H13" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H14" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="D15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="1" t="s">
+      <c r="D16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H16" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="E17" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>84</v>
+        <v>8</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="H17" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>60</v>
+        <v>3</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="H18" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>62</v>
+        <v>3</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="H19" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>64</v>
+        <v>21</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>65</v>
+        <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>66</v>
+        <v>3</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="H20" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>86</v>
+        <v>4</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>87</v>
+        <v>8</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>88</v>
+        <v>97</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="H21" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>89</v>
+        <v>51</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>90</v>
+        <v>4</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>91</v>
+        <v>8</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>93</v>
+        <v>29</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="H22" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>75</v>
+        <v>2</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>76</v>
+        <v>3</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>68</v>
+        <v>4</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="H23" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>58</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>94</v>
+        <v>3</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H25" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H26" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="E27" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>60</v>
+        <v>83</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="H27" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H28" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H29" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H30" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H31" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F32" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G32" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
@@ -1656,129 +1760,147 @@
       <c r="E33" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="1" t="s">
         <v>66</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>3</v>
+        <v>64</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>4</v>
+        <v>65</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>46</v>
+        <v>21</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="H34" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>3</v>
+        <v>86</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>43</v>
+        <v>76</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="H35" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>37</v>
+        <v>89</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>39</v>
+        <v>91</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>41</v>
+        <v>92</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="H36" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>2</v>
+        <v>75</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>3</v>
+        <v>76</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>5</v>
+        <v>77</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="H37" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>4</v>
+        <v>75</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>98</v>
+        <v>77</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="H38" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>0</v>
       </c>
@@ -1794,17 +1916,21 @@
       <c r="E39" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F39" s="1" t="s">
         <v>103</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>126</v>
       </c>
+      <c r="H39" s="2">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>